<commit_message>
T3 Finir le excel et ajuster le diagramme logique
</commit_message>
<xml_diff>
--- a/Travail 3/ListesAccess.xlsx
+++ b/Travail 3/ListesAccess.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\533\Desktop\Reseau2\Travail 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yannick\Desktop\Reseau2\Travail 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FD39CE-7229-4D0C-8DDB-F223B21F9B19}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="73">
   <si>
     <t>R_SS</t>
   </si>
@@ -225,13 +226,31 @@
   </si>
   <si>
     <t>TCP(HTTP)</t>
+  </si>
+  <si>
+    <t>R_E</t>
+  </si>
+  <si>
+    <t>192.168.12.0 /24</t>
+  </si>
+  <si>
+    <t>R_P</t>
+  </si>
+  <si>
+    <t>192.168.11.0 /24</t>
+  </si>
+  <si>
+    <t>192.168.21.0 /24</t>
+  </si>
+  <si>
+    <t>192.168.31.0 /24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +282,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,8 +334,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -411,11 +444,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -561,15 +603,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -577,6 +610,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,11 +921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,23 +941,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="51"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="58"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="48"/>
@@ -2104,8 +2167,1252 @@
         <v>31</v>
       </c>
     </row>
+    <row r="36" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A36" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="48"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
+      <c r="O37" s="48"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="48"/>
+      <c r="B38" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="54"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="52"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="48"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="L39" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="M39" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N39" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="M42" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="N42" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="42"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K43" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="M43" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="42"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H44" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I44" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K44" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L44" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="M44" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O44" s="44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="42"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H45" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J45" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="K45" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="M45" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N45" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O45" s="44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J46" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="K46" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L46" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="M46" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O46" s="44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="45"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I47" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="J47" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="K47" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="L47" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="M47" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="N47" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="O47" s="47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A51" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="55"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="55"/>
+      <c r="M51" s="55"/>
+      <c r="N51" s="55"/>
+      <c r="O51" s="55"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="48"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="K52" s="53"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="53"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="48"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="48"/>
+      <c r="B53" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="52"/>
+      <c r="G53" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" s="52"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="K53" s="50"/>
+      <c r="L53" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="48"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="H54" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="J54" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="K54" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="L54" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="M54" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="N54" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O54" s="48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N55" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O55" s="5"/>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="J57" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="60"/>
+      <c r="L57" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="M57" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="N57" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="O57" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="42"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I58" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J58" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="K58" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L58" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M58" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N58" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O58" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="42"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F59" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="H59" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I59" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J59" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="K59" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L59" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M59" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O59" s="44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="42"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="H60" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J60" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="K60" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L60" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M60" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N60" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O60" s="44" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="42"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="H61" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="I61" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J61" s="43" t="s">
+        <v>38</v>
+      </c>
+      <c r="K61" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L61" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="M61" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N61" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O61" s="44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="45"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="H62" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="J62" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="K62" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="L62" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="M62" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="N62" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="O62" s="47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E64" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J64" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K64" s="25"/>
+      <c r="L64" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="M64" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="N64" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="O64" s="26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="27"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E65" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H65" s="28">
+        <v>80</v>
+      </c>
+      <c r="I65" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="K65" s="28">
+        <v>80</v>
+      </c>
+      <c r="L65" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M65" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="N65" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="O65" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="27"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G66" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H66" s="28">
+        <v>53</v>
+      </c>
+      <c r="I66" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="K66" s="28">
+        <v>53</v>
+      </c>
+      <c r="L66" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M66" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="N66" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="O66" s="29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="27"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G67" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H67" s="28">
+        <v>25</v>
+      </c>
+      <c r="I67" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="K67" s="28">
+        <v>25</v>
+      </c>
+      <c r="L67" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="M67" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="N67" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="O67" s="29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="30"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H68" s="31">
+        <v>110</v>
+      </c>
+      <c r="I68" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="K68" s="31">
+        <v>110</v>
+      </c>
+      <c r="L68" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="M68" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N68" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="O68" s="32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="G70" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="H70" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I70" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="K70" s="34"/>
+      <c r="L70" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="M70" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N70" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="O70" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="36"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F71" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G71" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="37">
+        <v>25</v>
+      </c>
+      <c r="I71" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="K71" s="37">
+        <v>25</v>
+      </c>
+      <c r="L71" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="M71" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N71" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O71" s="38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="36"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F72" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G72" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H72" s="37">
+        <v>110</v>
+      </c>
+      <c r="I72" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J72" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="K72" s="37">
+        <v>110</v>
+      </c>
+      <c r="L72" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="M72" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N72" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O72" s="38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="36"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F73" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G73" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H73" s="37">
+        <v>53</v>
+      </c>
+      <c r="I73" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="J73" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="K73" s="37">
+        <v>53</v>
+      </c>
+      <c r="L73" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="M73" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="N73" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O73" s="38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="39"/>
+      <c r="B74" s="40"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E74" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F74" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G74" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H74" s="40">
+        <v>80</v>
+      </c>
+      <c r="I74" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="J74" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="K74" s="40">
+        <v>80</v>
+      </c>
+      <c r="L74" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="M74" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="N74" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="O74" s="41" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="18">
+    <mergeCell ref="A36:O36"/>
+    <mergeCell ref="A51:O51"/>
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="J52:N52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:N2"/>

</xml_diff>